<commit_message>
Initial commit of iOS project
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amparo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/OneDrive/Software Development/iOS/RSR-Pechhulp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_0B0D02570FDDAA2C71767F6E80C5EAE34283AC73" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3192972E-3FF1-4D49-8FD9-89361B5E234E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Subject</t>
   </si>
@@ -39,15 +45,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Implementing …</t>
-  </si>
-  <si>
-    <t>Example 2</t>
   </si>
   <si>
     <t>Had some issues with…</t>
@@ -77,11 +74,17 @@
   <si>
     <t>Total amount of hours</t>
   </si>
+  <si>
+    <t>Downloaded the live version of the app</t>
+  </si>
+  <si>
+    <t>Explored the already made app to inform my app</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -426,8 +429,8 @@
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Standaard 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1677,19 +1680,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
@@ -1702,9 +1705,9 @@
       <c r="E1" s="11"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="38.1" customHeight="1">
+    <row r="2" spans="1:6" ht="38" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1712,7 +1715,7 @@
       <c r="E2" s="22"/>
       <c r="F2" s="23"/>
     </row>
-    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:6" ht="17" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -1728,26 +1731,24 @@
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:6" ht="17" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="19">
-        <v>42736</v>
+        <v>43481</v>
       </c>
       <c r="C4" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="1:6" ht="17" customHeight="1">
+      <c r="A5" s="6"/>
       <c r="B5" s="19">
         <v>42736</v>
       </c>
@@ -1755,12 +1756,12 @@
         <v>0</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:6" ht="17" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="19"/>
       <c r="C6" s="18"/>
@@ -1768,7 +1769,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:6" ht="17" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="19"/>
       <c r="C7" s="18"/>
@@ -1776,7 +1777,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:6" ht="17" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="19"/>
       <c r="C8" s="18"/>
@@ -1784,7 +1785,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:6" ht="17" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="19"/>
       <c r="C9" s="18"/>
@@ -1792,7 +1793,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:6" ht="17" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="19"/>
       <c r="C10" s="18"/>
@@ -1800,7 +1801,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:6" ht="17" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="19"/>
       <c r="C11" s="18"/>
@@ -1808,7 +1809,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:6" ht="17" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="19"/>
       <c r="C12" s="18"/>
@@ -1816,7 +1817,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:6" ht="17" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="19"/>
       <c r="C13" s="18"/>
@@ -1824,7 +1825,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:6" ht="17" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="19"/>
       <c r="C14" s="18"/>
@@ -1832,7 +1833,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:6" ht="17" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="19"/>
       <c r="C15" s="18"/>
@@ -1840,7 +1841,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:6" ht="17" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="19"/>
       <c r="C16" s="18"/>
@@ -1848,7 +1849,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:6" ht="17" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="19"/>
       <c r="C17" s="18"/>
@@ -1856,7 +1857,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:6" ht="17" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="19"/>
       <c r="C18" s="18"/>
@@ -1864,7 +1865,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:6" ht="17" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="19"/>
       <c r="C19" s="18"/>
@@ -1872,7 +1873,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:6" ht="17" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="19"/>
       <c r="C20" s="18"/>
@@ -1880,7 +1881,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:6" ht="17" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="19"/>
       <c r="C21" s="18"/>
@@ -1888,7 +1889,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:6" ht="17" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="19"/>
       <c r="C22" s="18"/>
@@ -1896,7 +1897,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:6" ht="17" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="19"/>
       <c r="C23" s="18"/>
@@ -1904,7 +1905,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:6" ht="17" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="19"/>
       <c r="C24" s="18"/>
@@ -1912,7 +1913,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:6" ht="17" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="19"/>
       <c r="C25" s="18"/>
@@ -1920,7 +1921,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:6" ht="17" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="19"/>
       <c r="C26" s="18"/>
@@ -1928,7 +1929,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:6" ht="17" customHeight="1">
       <c r="A27" s="6"/>
       <c r="B27" s="19"/>
       <c r="C27" s="18"/>
@@ -1936,7 +1937,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:6" ht="17" customHeight="1">
       <c r="A28" s="6"/>
       <c r="B28" s="19"/>
       <c r="C28" s="18"/>
@@ -1944,7 +1945,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="15.95" customHeight="1">
+    <row r="29" spans="1:6" ht="16" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1952,20 +1953,20 @@
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="15.95" customHeight="1">
+    <row r="30" spans="1:6" ht="16" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B30" s="15">
         <f>SUM(C4:C28)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="15.95" customHeight="1">
+    <row r="31" spans="1:6" ht="16" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1973,7 +1974,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="15.95" customHeight="1">
+    <row r="32" spans="1:6" ht="16" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1981,7 +1982,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15.95" customHeight="1">
+    <row r="33" spans="1:6" ht="16" customHeight="1">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>

</xml_diff>

<commit_message>
Setup basic UI and added resources
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/OneDrive/Software Development/iOS/RSR-Pechhulp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_0B0D02570FDDAA2C71767F6E80C5EAE34283AC73" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3192972E-3FF1-4D49-8FD9-89361B5E234E}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_0B0D02570FDDAA2C71767F6E80C5EAE34283AC73" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B181B8F6-B869-0A47-9635-9DF753463D4D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Subject</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
   </si>
   <si>
     <r>
@@ -1707,7 +1704,7 @@
     </row>
     <row r="2" spans="1:6" ht="38" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1733,7 +1730,7 @@
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="19">
         <v>43481</v>
@@ -1742,22 +1739,16 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="17" customHeight="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="19">
-        <v>42736</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>4</v>
-      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="3"/>
       <c r="F5" s="5"/>
     </row>
@@ -1955,7 +1946,7 @@
     </row>
     <row r="30" spans="1:6" ht="16" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="15">
         <f>SUM(C4:C28)</f>

</xml_diff>